<commit_message>
Pós reunião Gustavo Código funcionando!
</commit_message>
<xml_diff>
--- a/debug.xlsx
+++ b/debug.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F17935-D759-4FDC-9D85-3EDD94CDE099}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04056C21-B4DA-4EC8-8644-7FA325E2DCC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Duvidas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>k =</t>
   </si>
@@ -85,6 +86,21 @@
   </si>
   <si>
     <t>Multiplicando os valores de rho e cv</t>
+  </si>
+  <si>
+    <t>Passando valores para ouro lado de novo</t>
+  </si>
+  <si>
+    <t>10.0 / 0.0</t>
+  </si>
+  <si>
+    <t>duvidas</t>
+  </si>
+  <si>
+    <t>Equacionamento</t>
+  </si>
+  <si>
+    <t>Tenho que multiplicar as ccs por dt?</t>
   </si>
 </sst>
 </file>
@@ -126,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,6 +154,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -421,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +454,7 @@
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -444,13 +463,13 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="2"/>
@@ -462,7 +481,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -471,7 +490,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +507,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -510,7 +529,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -533,7 +552,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -554,14 +573,14 @@
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -581,12 +600,15 @@
       <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="Q8">
+        <v>24.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -606,14 +628,14 @@
       <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -632,14 +654,14 @@
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -659,22 +681,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -694,7 +716,7 @@
         <v>32908.61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -714,21 +736,24 @@
         <v>329092.06</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="2">
-        <v>100000</v>
+      <c r="D15" s="3">
+        <v>10000</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -743,4 +768,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F618CD7F-62C3-44F6-B649-3C880D86C7D5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>